<commit_message>
Begin changing the dropdown named ranges in the 'Information Sales' tab to dynamic ranges via offset functions
</commit_message>
<xml_diff>
--- a/Quote Template.xlsx
+++ b/Quote Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8505" yWindow="105" windowWidth="8325" windowHeight="8055" tabRatio="740" activeTab="3"/>
+    <workbookView xWindow="8505" yWindow="105" windowWidth="8325" windowHeight="8055" tabRatio="740"/>
   </bookViews>
   <sheets>
     <sheet name="Information Sales" sheetId="12" r:id="rId1"/>
@@ -25,13 +25,14 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'PARTS LIST SC'!$1:$10</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'TASK LIST SC'!$1:$5</definedName>
+    <definedName name="QuoteType">OFFSET(Sheet2!$B$2,0,0,COUNTA(Sheet2!$B:$B)-1,1)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="436">
   <si>
     <t>PARTS LIST</t>
   </si>
@@ -3341,8 +3342,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N81"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3456,9 +3457,7 @@
         <v>130</v>
       </c>
       <c r="J6" s="235"/>
-      <c r="K6" s="230" t="s">
-        <v>329</v>
-      </c>
+      <c r="K6" s="230"/>
       <c r="L6" s="230"/>
       <c r="M6" s="230"/>
       <c r="N6" s="230"/>
@@ -4849,17 +4848,16 @@
     <mergeCell ref="K8:N8"/>
     <mergeCell ref="K9:N9"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:N6">
+      <formula1>QuoteType</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Sheet1!$B$3:$B$42</xm:f>
-          </x14:formula1>
-          <xm:sqref>K6:N6</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$E:$E</xm:f>
@@ -7471,7 +7469,7 @@
   </sheetPr>
   <dimension ref="B1:T123"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -19633,7 +19631,7 @@
   <dimension ref="B1:R160"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B41"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20671,7 +20669,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="B2:B43"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>